<commit_message>
refactor and add pdf support
</commit_message>
<xml_diff>
--- a/tmp/3SECONDES/3SECONDES.doc-total-recap.xlsx
+++ b/tmp/3SECONDES/3SECONDES.doc-total-recap.xlsx
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,167 +537,167 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>5 - OFFICIAL 1</t>
+          <t>5 - HEAD OF SPORTS COMMITTEE</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>6 - KSENIA</t>
+          <t>6 - OFFICIAL 1</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>7 - OFFICIAL 2</t>
+          <t>7 - KSENIA</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>8 - PAULAUSKAS</t>
+          <t>8 - OFFICIAL 2</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>49</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>9 - GOMELKIY</t>
+          <t>9 - PAULAUSKAS</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>10 - ALEXANDER BELOV</t>
+          <t>10 - GOMELKIY</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>11 - KORKIYA</t>
+          <t>11 - ALEXANDER BELOV</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>12 - EDESHKO</t>
+          <t>12 - KORKIYA</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>13 - SAKANDELIDZE</t>
+          <t>13 - EDESHKO</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>14 - ZHARMUKHAMEDOV</t>
+          <t>14 - SAKANDELIDZE</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>15 - SERGEY BELOV</t>
+          <t>15 - ZHARMUKHAMEDOV</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>42</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>16 - PLAYER</t>
+          <t>16 - SERGEY BELOV</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>17 - DOCTOR</t>
+          <t>17 - PLAYER</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18 - PLAYERS</t>
+          <t>18 - DOCTOR</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19 - TRANSLATOR</t>
+          <t>19 - PLAYERS</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20 - TEAM</t>
+          <t>20 - TRANSLATOR</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>21 - PASSAGE</t>
+          <t>21 - TEAM</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -707,47 +707,47 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>22 - AIRPORT WORKER 1</t>
+          <t>22 - PASSAGE</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>23 - CHAYKIN</t>
+          <t>23 - AIRPORT WORKER 1</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>24 - CUSTOMER-FAN</t>
+          <t>24 - CHAYKIN</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>25 - CUSTOMER 1</t>
+          <t>25 - CUSTOMER-FAN</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>26 - CUSTOMER 2</t>
+          <t>26 - CUSTOMER 1</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -757,37 +757,37 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>27 - KSENIYA</t>
+          <t>27 - CUSTOMER 2</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>28 - TRAINER</t>
+          <t>28 - KSENIYA</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>29 - POLYAKOVA</t>
+          <t>29 - TRAINER</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>30 - SURKOVA</t>
+          <t>30 - POLYAKOVA</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -797,7 +797,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>31 - CANARIS</t>
+          <t>31 - SURKOVA</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -807,7 +807,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>32 - SMIRNOVA</t>
+          <t>32 - CANARIS</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -817,7 +817,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>33 - NIKOLAYEVA</t>
+          <t>33 - SMIRNOVA</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -827,27 +827,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>34 - SVESHNIKOVA</t>
+          <t>34 - NIKOLAYEVA</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>35 - VLASOVA</t>
+          <t>35 - SVESHNIKOVA</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>36 - SPORTSWOMAN</t>
+          <t>36 - VLASOVA</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -857,27 +857,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>37 - SASHA BELOV</t>
+          <t>37 - SPORTSWOMAN</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>38 - EDESHKO/ZHARMUKHAMEDOV/BELOV</t>
+          <t>38 - SASHA BELOV</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>39 - VOLNOV</t>
+          <t>39 - EDESHKO/ZHARMUKHAMEDOV/BELOV</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -887,7 +887,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>40 - TAXI DRIVER</t>
+          <t>40 - VOLNOV</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -897,87 +897,87 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>41 - UNCLE ILIKO</t>
+          <t>41 - TAXI DRIVER</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>42 - VOLNOV’S WIFE</t>
+          <t>42 - UNCLE ILIKO</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>43 - EDESHKO’S GIRLFRIEND</t>
+          <t>43 - VOLNOV’S WIFE</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>44 - WOMAN</t>
+          <t>44 - EDESHKO’S GIRLFRIEND</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>45 - REPORTER</t>
+          <t>45 - WOMAN</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>46 - VSEVOLOD</t>
+          <t>46 - REPORTER</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>47 - LITHUANIAN REPORTER</t>
+          <t>47 - VSEVOLOD</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>48 - VLEVOLOD</t>
+          <t>48 - LITHUANIAN REPORTER</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>49 - CUBAN</t>
+          <t>49 - VLEVOLOD</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -987,67 +987,67 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>50 - LITHUANIAN DRIVER</t>
+          <t>50 - CUBAN</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>51 - DRIVER</t>
+          <t>51 - LITHUANIAN DRIVER</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>52 - LITHUANIAN TOURIST</t>
+          <t>52 - DRIVER</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>53 - BRUNDAGE’S VOICE</t>
+          <t>53 - LITHUANIAN TOURIST</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>54 - MEDIC</t>
+          <t>54 - BRUNDAGE’S VOICE</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>55 - INTERPRETER</t>
+          <t>55 - MEDIC</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>56 - ADMINISTRATOR</t>
+          <t>56 - INTERPRETER</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1057,37 +1057,37 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>57 - ANNOUNCER</t>
+          <t>57 - ADMINISTRATOR</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>58 - SERGEY PAVLOVICH</t>
+          <t>58 - ANNOUNCER</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>59 - REFEREE</t>
+          <t>59 - SERGEY PAVLOVICH</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>60 - AKSAKAL</t>
+          <t>60 - REFEREE</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1097,7 +1097,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>61 - SPECTATORS</t>
+          <t>61 - AKSAKAL</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1107,17 +1107,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>62 - GRANDFATHER</t>
+          <t>62 - SPECTATORS</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>63 - BASKETBALL PLAYER</t>
+          <t>63 - GRANDFATHER</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1127,37 +1127,37 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>64 - GALYA</t>
+          <t>64 - BASKETBALL PLAYER</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>65 - YERYOMINA</t>
+          <t>65 - GALYA</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>66 - MALE VOICE</t>
+          <t>66 - YERYOMINA</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>67 - AUNT KORKIYA</t>
+          <t>67 - MALE VOICE</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1167,27 +1167,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>68 - FANS</t>
+          <t>68 - AUNT KORKIYA</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>69 - NOT IDENTIFIED</t>
+          <t>69 - FANS</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>70 - ANATOLIY</t>
+          <t>70 - NOT IDENTIFIED</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1197,10 +1197,20 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>71 - YEREMINA</t>
+          <t>71 - ANATOLIY</t>
         </is>
       </c>
       <c r="B74" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>72 - YEREMINA</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>